<commit_message>
nuovi # di maglia
</commit_message>
<xml_diff>
--- a/data/Rosa e Stats 2020-2021.xlsx
+++ b/data/Rosa e Stats 2020-2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/totti/Developer/fun/tamarindi-web/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{13B7B3F3-D70A-1D46-86E3-6DBD50578131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{EC8CE34D-91C5-D640-9B03-8B413D2F5FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="620" windowWidth="18740" windowHeight="11700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,8 +19,8 @@
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
+    <customWorkbookView name="Acer - Visualizzazione personale" guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="802" activeSheetId="1"/>
     <customWorkbookView name="Matteo Cutroni - Personal View" guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}" mergeInterval="0" personalView="1" xWindow="18" yWindow="31" windowWidth="937" windowHeight="585" activeSheetId="1"/>
-    <customWorkbookView name="Acer - Visualizzazione personale" guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1916" windowHeight="802" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="128">
   <si>
     <t>TAMARINDI F.C. 2020-2021</t>
   </si>
@@ -421,6 +421,9 @@
   <si>
     <t>Coddetta [P]</t>
   </si>
+  <si>
+    <t>13</t>
+  </si>
 </sst>
 </file>
 
@@ -523,10 +526,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +550,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{BA0E6AD0-F03D-024F-B6B0-768153E5143B}" diskRevisions="1" revisionId="351" version="37">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F71431B5-F5BD-8445-9B0B-7C45DA8470D0}" diskRevisions="1" revisionId="356" version="38">
   <header guid="{BA0E6AD0-F03D-024F-B6B0-768153E5143B}" dateTime="2025-11-18T23:59:00" maxSheetId="4" userName="Matteo Cutroni" r:id="rId37" minRId="349" maxRId="351">
     <sheetIdMap count="3">
       <sheetId val="1"/>
@@ -553,7 +558,51 @@
       <sheetId val="3"/>
     </sheetIdMap>
   </header>
+  <header guid="{F71431B5-F5BD-8445-9B0B-7C45DA8470D0}" dateTime="2025-11-19T01:12:12" maxSheetId="4" userName="Matteo Cutroni" r:id="rId38" minRId="352" maxRId="356">
+    <sheetIdMap count="3">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+    </sheetIdMap>
+  </header>
 </headers>
+</file>
+
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="352" sId="1">
+    <nc r="D13" t="inlineStr">
+      <is>
+        <t>13</t>
+      </is>
+    </nc>
+  </rcc>
+  <rfmt sheetId="1" sqref="D13">
+    <dxf>
+      <alignment horizontal="right"/>
+    </dxf>
+  </rfmt>
+  <rcc rId="353" sId="1">
+    <nc r="D17">
+      <v>23</v>
+    </nc>
+  </rcc>
+  <rcc rId="354" sId="1">
+    <nc r="D22">
+      <v>34</v>
+    </nc>
+  </rcc>
+  <rcc rId="355" sId="1">
+    <nc r="D25">
+      <v>24</v>
+    </nc>
+  </rcc>
+  <rcc rId="356" sId="1">
+    <nc r="D34">
+      <v>56</v>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -891,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BZ265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="A24" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1217,7 +1266,7 @@
       <c r="BY4" s="1"/>
       <c r="BZ4" s="1"/>
     </row>
-    <row r="5" spans="1:78" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:78" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
@@ -1254,7 +1303,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:78" s="3" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:78" s="3" customFormat="1" ht="12" x14ac:dyDescent="0.15">
       <c r="F6" s="4" t="s">
         <v>6</v>
       </c>
@@ -1880,7 +1929,9 @@
       </c>
       <c r="B13" s="11"/>
       <c r="C13" s="11"/>
-      <c r="D13" s="15"/>
+      <c r="D13" s="18" t="s">
+        <v>127</v>
+      </c>
       <c r="E13" s="11"/>
       <c r="F13" s="11">
         <v>1</v>
@@ -2266,7 +2317,9 @@
       </c>
       <c r="B17" s="11"/>
       <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="11">
+        <v>23</v>
+      </c>
       <c r="E17" s="11"/>
       <c r="F17" s="11">
         <v>1</v>
@@ -2763,7 +2816,9 @@
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
+      <c r="D22" s="1">
+        <v>34</v>
+      </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1">
@@ -3066,7 +3121,9 @@
       </c>
       <c r="B25" s="11"/>
       <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
+      <c r="D25" s="11">
+        <v>24</v>
+      </c>
       <c r="E25" s="11"/>
       <c r="F25" s="11">
         <v>1</v>
@@ -3775,106 +3832,106 @@
       <c r="BY31" s="1"/>
       <c r="BZ31" s="1"/>
     </row>
-    <row r="32" spans="1:78" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16" t="s">
+    <row r="32" spans="1:78" s="16" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16">
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15">
         <v>31</v>
       </c>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16">
+      <c r="E32" s="15"/>
+      <c r="F32" s="15">
         <v>2</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16">
+      <c r="G32" s="15"/>
+      <c r="H32" s="15">
         <f>SUM(F32:G32)</f>
         <v>2</v>
       </c>
-      <c r="I32" s="16"/>
-      <c r="J32" s="16"/>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16">
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15">
         <f>SUM(J32:L32)</f>
         <v>0</v>
       </c>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="16"/>
-      <c r="T32" s="16" t="s">
+      <c r="N32" s="15"/>
+      <c r="O32" s="15"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
+      <c r="S32" s="15"/>
+      <c r="T32" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="U32" s="16"/>
-      <c r="V32" s="16" t="s">
+      <c r="U32" s="15"/>
+      <c r="V32" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="W32" s="16"/>
-      <c r="Z32" s="18">
+      <c r="W32" s="15"/>
+      <c r="Z32" s="17">
         <v>36581</v>
       </c>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="16">
+      <c r="AA32" s="15"/>
+      <c r="AB32" s="15">
         <v>6</v>
       </c>
-      <c r="AC32" s="16">
+      <c r="AC32" s="15">
         <f>SUM(AB32,M32)</f>
         <v>6</v>
       </c>
-      <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16"/>
-      <c r="AG32" s="16"/>
-      <c r="AH32" s="16"/>
-      <c r="AI32" s="16"/>
-      <c r="AJ32" s="16"/>
-      <c r="AK32" s="16"/>
-      <c r="AL32" s="16"/>
-      <c r="AM32" s="16"/>
-      <c r="AN32" s="16"/>
-      <c r="AO32" s="16"/>
-      <c r="AP32" s="16"/>
-      <c r="AQ32" s="16"/>
-      <c r="AR32" s="16"/>
-      <c r="AS32" s="16"/>
-      <c r="AT32" s="16"/>
-      <c r="AU32" s="16"/>
-      <c r="AV32" s="16"/>
-      <c r="AW32" s="16"/>
-      <c r="AX32" s="16"/>
-      <c r="AY32" s="16"/>
-      <c r="AZ32" s="16"/>
-      <c r="BA32" s="16"/>
-      <c r="BB32" s="16"/>
-      <c r="BC32" s="16"/>
-      <c r="BD32" s="16"/>
-      <c r="BE32" s="16"/>
-      <c r="BF32" s="16"/>
-      <c r="BG32" s="16"/>
-      <c r="BH32" s="16"/>
-      <c r="BI32" s="16"/>
-      <c r="BJ32" s="16"/>
-      <c r="BK32" s="16"/>
-      <c r="BL32" s="16"/>
-      <c r="BM32" s="16"/>
-      <c r="BN32" s="16"/>
-      <c r="BO32" s="16"/>
-      <c r="BP32" s="16"/>
-      <c r="BQ32" s="16"/>
-      <c r="BR32" s="16"/>
-      <c r="BS32" s="16"/>
-      <c r="BT32" s="16"/>
-      <c r="BU32" s="16"/>
-      <c r="BV32" s="16"/>
-      <c r="BW32" s="16"/>
-      <c r="BX32" s="16"/>
-      <c r="BY32" s="16"/>
-      <c r="BZ32" s="16"/>
+      <c r="AD32" s="15"/>
+      <c r="AE32" s="15"/>
+      <c r="AF32" s="15"/>
+      <c r="AG32" s="15"/>
+      <c r="AH32" s="15"/>
+      <c r="AI32" s="15"/>
+      <c r="AJ32" s="15"/>
+      <c r="AK32" s="15"/>
+      <c r="AL32" s="15"/>
+      <c r="AM32" s="15"/>
+      <c r="AN32" s="15"/>
+      <c r="AO32" s="15"/>
+      <c r="AP32" s="15"/>
+      <c r="AQ32" s="15"/>
+      <c r="AR32" s="15"/>
+      <c r="AS32" s="15"/>
+      <c r="AT32" s="15"/>
+      <c r="AU32" s="15"/>
+      <c r="AV32" s="15"/>
+      <c r="AW32" s="15"/>
+      <c r="AX32" s="15"/>
+      <c r="AY32" s="15"/>
+      <c r="AZ32" s="15"/>
+      <c r="BA32" s="15"/>
+      <c r="BB32" s="15"/>
+      <c r="BC32" s="15"/>
+      <c r="BD32" s="15"/>
+      <c r="BE32" s="15"/>
+      <c r="BF32" s="15"/>
+      <c r="BG32" s="15"/>
+      <c r="BH32" s="15"/>
+      <c r="BI32" s="15"/>
+      <c r="BJ32" s="15"/>
+      <c r="BK32" s="15"/>
+      <c r="BL32" s="15"/>
+      <c r="BM32" s="15"/>
+      <c r="BN32" s="15"/>
+      <c r="BO32" s="15"/>
+      <c r="BP32" s="15"/>
+      <c r="BQ32" s="15"/>
+      <c r="BR32" s="15"/>
+      <c r="BS32" s="15"/>
+      <c r="BT32" s="15"/>
+      <c r="BU32" s="15"/>
+      <c r="BV32" s="15"/>
+      <c r="BW32" s="15"/>
+      <c r="BX32" s="15"/>
+      <c r="BY32" s="15"/>
+      <c r="BZ32" s="15"/>
     </row>
     <row r="33" spans="1:78" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
@@ -3981,7 +4038,9 @@
       </c>
       <c r="B34" s="11"/>
       <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
+      <c r="D34" s="11">
+        <v>56</v>
+      </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11">
         <v>1</v>
@@ -22588,13 +22647,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}" topLeftCell="A32">
-      <selection activeCell="F70" sqref="F70"/>
+    <customSheetView guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}" topLeftCell="A5">
+      <selection activeCell="I47" sqref="I47"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}" topLeftCell="A5">
-      <selection activeCell="I47" sqref="I47"/>
+    <customSheetView guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}" topLeftCell="A32">
+      <selection activeCell="F70" sqref="F70"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -22615,12 +22674,12 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}" topLeftCell="A116">
-      <selection activeCell="E138" sqref="E138"/>
+    <customSheetView guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
     </customSheetView>
-    <customSheetView guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}">
+    <customSheetView guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}" topLeftCell="A116">
+      <selection activeCell="E138" sqref="E138"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
     </customSheetView>
@@ -22639,11 +22698,11 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <customSheetViews>
-    <customSheetView guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}">
+    <customSheetView guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
     </customSheetView>
-    <customSheetView guid="{732A3E98-21F1-4683-8627-B42F20E3CD9F}">
+    <customSheetView guid="{BDA24EDC-855E-3043-8B0E-6E43ED6DDC1A}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
     </customSheetView>

</xml_diff>